<commit_message>
Atualizacao no cronograma e recursos humanos
</commit_message>
<xml_diff>
--- a/Artefatos de Documentação/Processo Aplicado/EveRemind/2-Gerencia de Projeto/Templates/Cronograma.xlsx
+++ b/Artefatos de Documentação/Processo Aplicado/EveRemind/2-Gerencia de Projeto/Templates/Cronograma.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="123820"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="25808"/>
+  <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leonardo\Dropbox\Engenharia de Software\5º Periodo\Trabalho Multidisciplinar\Repositório\P.I.-ES-UFG-2015-BIJLMMV\Artefatos de Documentação\Processo Genérico\2-Gerencia de Projeto\Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/viniciuscmac/Desktop/GitHub/P.I.-ES-UFG-2015-BIJLMMV/Artefatos de Documentação/Processo Aplicado/EveRemind/2-Gerencia de Projeto/Templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25760" windowHeight="15480"/>
   </bookViews>
   <sheets>
     <sheet name="Cronograma" sheetId="4" r:id="rId1"/>
@@ -35,13 +35,18 @@
     <definedName name="Urgencia" localSheetId="1">#REF!</definedName>
     <definedName name="Urgencia">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <webPublishing codePage="1252"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
   <si>
     <t>Atividade</t>
   </si>
@@ -89,6 +94,21 @@
   </si>
   <si>
     <t>Dependências</t>
+  </si>
+  <si>
+    <t>Área de Processo</t>
+  </si>
+  <si>
+    <t>Esforço da Atividade</t>
+  </si>
+  <si>
+    <t>Recursos Ambientais</t>
+  </si>
+  <si>
+    <t>Recursos Humanos</t>
+  </si>
+  <si>
+    <t>Custo Estimado</t>
   </si>
 </sst>
 </file>
@@ -482,16 +502,16 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -715,64 +735,64 @@
     </xf>
   </cellXfs>
   <cellStyles count="58">
-    <cellStyle name="Accent1" xfId="1" builtinId="29" customBuiltin="1"/>
     <cellStyle name="Accent1 - 20%" xfId="2"/>
     <cellStyle name="Accent1 - 20% 2" xfId="45"/>
     <cellStyle name="Accent1 - 40%" xfId="3"/>
     <cellStyle name="Accent1 - 40% 2" xfId="46"/>
     <cellStyle name="Accent1 - 60%" xfId="4"/>
-    <cellStyle name="Accent2" xfId="5" builtinId="33" customBuiltin="1"/>
     <cellStyle name="Accent2 - 20%" xfId="6"/>
     <cellStyle name="Accent2 - 20% 2" xfId="47"/>
     <cellStyle name="Accent2 - 40%" xfId="7"/>
     <cellStyle name="Accent2 - 40% 2" xfId="48"/>
     <cellStyle name="Accent2 - 60%" xfId="8"/>
-    <cellStyle name="Accent3" xfId="9" builtinId="37" customBuiltin="1"/>
     <cellStyle name="Accent3 - 20%" xfId="10"/>
     <cellStyle name="Accent3 - 20% 2" xfId="49"/>
     <cellStyle name="Accent3 - 40%" xfId="11"/>
     <cellStyle name="Accent3 - 40% 2" xfId="50"/>
     <cellStyle name="Accent3 - 60%" xfId="12"/>
-    <cellStyle name="Accent4" xfId="13" builtinId="41" customBuiltin="1"/>
     <cellStyle name="Accent4 - 20%" xfId="14"/>
     <cellStyle name="Accent4 - 20% 2" xfId="51"/>
     <cellStyle name="Accent4 - 40%" xfId="15"/>
     <cellStyle name="Accent4 - 40% 2" xfId="52"/>
     <cellStyle name="Accent4 - 60%" xfId="16"/>
-    <cellStyle name="Accent5" xfId="17" builtinId="45" customBuiltin="1"/>
     <cellStyle name="Accent5 - 20%" xfId="18"/>
     <cellStyle name="Accent5 - 20% 2" xfId="53"/>
     <cellStyle name="Accent5 - 40%" xfId="19"/>
     <cellStyle name="Accent5 - 40% 2" xfId="54"/>
     <cellStyle name="Accent5 - 60%" xfId="20"/>
-    <cellStyle name="Accent6" xfId="21" builtinId="49" customBuiltin="1"/>
     <cellStyle name="Accent6 - 20%" xfId="22"/>
     <cellStyle name="Accent6 - 20% 2" xfId="55"/>
     <cellStyle name="Accent6 - 40%" xfId="23"/>
     <cellStyle name="Accent6 - 40% 2" xfId="56"/>
     <cellStyle name="Accent6 - 60%" xfId="24"/>
-    <cellStyle name="Bad" xfId="25" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="26" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="27" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Bom" xfId="31" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Cálculo" xfId="26" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Célula Vinculada" xfId="37" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Emphasis 1" xfId="28"/>
     <cellStyle name="Emphasis 2" xfId="29"/>
     <cellStyle name="Emphasis 3" xfId="30"/>
-    <cellStyle name="Good" xfId="31" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="32" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="33" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="34" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="35" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="36" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="37" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="38" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Ênfase1" xfId="1" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Ênfase2" xfId="5" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Ênfase3" xfId="9" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Ênfase4" xfId="13" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Ênfase5" xfId="17" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Ênfase6" xfId="21" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Entrada" xfId="36" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Incorreto" xfId="25" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Neutra" xfId="38" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="44"/>
-    <cellStyle name="Note" xfId="39" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="40" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Observação" xfId="39" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Percent 2" xfId="57"/>
+    <cellStyle name="Saída" xfId="40" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Sheet Title" xfId="41"/>
+    <cellStyle name="Texto de Aviso" xfId="43" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Título 1" xfId="32" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Título 2" xfId="33" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Título 3" xfId="34" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Título 4" xfId="35" builtinId="19" customBuiltin="1"/>
     <cellStyle name="Total" xfId="42" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="43" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Verificar Célula" xfId="27" builtinId="23" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="75">
     <dxf>
@@ -1462,7 +1482,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1745,34 +1765,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:H23"/>
+  <dimension ref="B1:J23"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="7.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="36.28515625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="15.42578125" style="4" customWidth="1"/>
-    <col min="7" max="7" width="19.85546875" style="4" customWidth="1"/>
-    <col min="8" max="8" width="25.42578125" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="8.83203125" style="1"/>
+    <col min="2" max="2" width="18.1640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="18.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="36.33203125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5" style="4" customWidth="1"/>
+    <col min="7" max="9" width="19.83203125" style="4" customWidth="1"/>
+    <col min="10" max="10" width="25.5" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C1" s="3"/>
       <c r="E1" s="5"/>
       <c r="G1" s="5"/>
-      <c r="H1" s="6"/>
-    </row>
-    <row r="2" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="6"/>
+    </row>
+    <row r="2" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="16" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C2" s="11" t="s">
         <v>0</v>
@@ -1787,22 +1809,30 @@
         <v>3</v>
       </c>
       <c r="G2" s="11" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
-      <c r="H2" s="10" t="s">
-        <v>15</v>
+      <c r="H2" s="11" t="s">
+        <v>19</v>
       </c>
-    </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I2" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" s="10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B3" s="2"/>
       <c r="C3" s="13"/>
       <c r="D3" s="12"/>
       <c r="E3" s="13"/>
       <c r="F3" s="14"/>
       <c r="G3" s="14"/>
-      <c r="H3" s="13"/>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="13"/>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B4" s="2"/>
       <c r="C4" s="14"/>
       <c r="D4" s="12"/>
@@ -1810,8 +1840,10 @@
       <c r="F4" s="14"/>
       <c r="G4" s="14"/>
       <c r="H4" s="14"/>
-    </row>
-    <row r="5" spans="2:8" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
+    </row>
+    <row r="5" spans="2:10" s="7" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B5" s="15"/>
       <c r="C5" s="14"/>
       <c r="D5" s="12"/>
@@ -1819,8 +1851,10 @@
       <c r="F5" s="14"/>
       <c r="G5" s="14"/>
       <c r="H5" s="14"/>
-    </row>
-    <row r="6" spans="2:8" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
+    </row>
+    <row r="6" spans="2:10" s="7" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B6" s="15"/>
       <c r="C6" s="14"/>
       <c r="D6" s="12"/>
@@ -1828,8 +1862,10 @@
       <c r="F6" s="14"/>
       <c r="G6" s="14"/>
       <c r="H6" s="14"/>
-    </row>
-    <row r="7" spans="2:8" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+    </row>
+    <row r="7" spans="2:10" s="7" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B7" s="15"/>
       <c r="C7" s="14"/>
       <c r="D7" s="12"/>
@@ -1837,8 +1873,10 @@
       <c r="F7" s="14"/>
       <c r="G7" s="14"/>
       <c r="H7" s="14"/>
-    </row>
-    <row r="8" spans="2:8" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
+    </row>
+    <row r="8" spans="2:10" s="7" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B8" s="15"/>
       <c r="C8" s="14"/>
       <c r="D8" s="12"/>
@@ -1846,8 +1884,10 @@
       <c r="F8" s="14"/>
       <c r="G8" s="14"/>
       <c r="H8" s="14"/>
-    </row>
-    <row r="9" spans="2:8" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+    </row>
+    <row r="9" spans="2:10" s="7" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B9" s="15"/>
       <c r="C9" s="14"/>
       <c r="D9" s="12"/>
@@ -1855,8 +1895,10 @@
       <c r="F9" s="14"/>
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
-    </row>
-    <row r="10" spans="2:8" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I9" s="14"/>
+      <c r="J9" s="14"/>
+    </row>
+    <row r="10" spans="2:10" s="7" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B10" s="15"/>
       <c r="C10" s="14"/>
       <c r="D10" s="12"/>
@@ -1864,8 +1906,10 @@
       <c r="F10" s="14"/>
       <c r="G10" s="14"/>
       <c r="H10" s="14"/>
-    </row>
-    <row r="11" spans="2:8" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I10" s="14"/>
+      <c r="J10" s="14"/>
+    </row>
+    <row r="11" spans="2:10" s="7" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B11" s="15"/>
       <c r="C11" s="14"/>
       <c r="D11" s="12"/>
@@ -1873,8 +1917,10 @@
       <c r="F11" s="14"/>
       <c r="G11" s="14"/>
       <c r="H11" s="14"/>
-    </row>
-    <row r="12" spans="2:8" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I11" s="14"/>
+      <c r="J11" s="14"/>
+    </row>
+    <row r="12" spans="2:10" s="7" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B12" s="15"/>
       <c r="C12" s="14"/>
       <c r="D12" s="12"/>
@@ -1882,8 +1928,10 @@
       <c r="F12" s="14"/>
       <c r="G12" s="14"/>
       <c r="H12" s="14"/>
-    </row>
-    <row r="13" spans="2:8" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I12" s="14"/>
+      <c r="J12" s="14"/>
+    </row>
+    <row r="13" spans="2:10" s="7" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B13" s="15"/>
       <c r="C13" s="14"/>
       <c r="D13" s="12"/>
@@ -1891,8 +1939,10 @@
       <c r="F13" s="14"/>
       <c r="G13" s="14"/>
       <c r="H13" s="14"/>
-    </row>
-    <row r="14" spans="2:8" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I13" s="14"/>
+      <c r="J13" s="14"/>
+    </row>
+    <row r="14" spans="2:10" s="7" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B14" s="15"/>
       <c r="C14" s="14"/>
       <c r="D14" s="12"/>
@@ -1900,8 +1950,10 @@
       <c r="F14" s="14"/>
       <c r="G14" s="14"/>
       <c r="H14" s="14"/>
-    </row>
-    <row r="15" spans="2:8" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I14" s="14"/>
+      <c r="J14" s="14"/>
+    </row>
+    <row r="15" spans="2:10" s="7" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B15" s="15"/>
       <c r="C15" s="14"/>
       <c r="D15" s="12"/>
@@ -1909,8 +1961,10 @@
       <c r="F15" s="14"/>
       <c r="G15" s="14"/>
       <c r="H15" s="14"/>
-    </row>
-    <row r="16" spans="2:8" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
+    </row>
+    <row r="16" spans="2:10" s="7" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B16" s="15"/>
       <c r="C16" s="14"/>
       <c r="D16" s="12"/>
@@ -1918,8 +1972,10 @@
       <c r="F16" s="14"/>
       <c r="G16" s="14"/>
       <c r="H16" s="14"/>
-    </row>
-    <row r="17" spans="2:8" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I16" s="14"/>
+      <c r="J16" s="14"/>
+    </row>
+    <row r="17" spans="2:10" s="7" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B17" s="15"/>
       <c r="C17" s="14"/>
       <c r="D17" s="12"/>
@@ -1927,18 +1983,22 @@
       <c r="F17" s="14"/>
       <c r="G17" s="14"/>
       <c r="H17" s="14"/>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I17" s="14"/>
+      <c r="J17" s="14"/>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.2">
       <c r="D18" s="8"/>
       <c r="E18" s="7"/>
       <c r="F18" s="8"/>
       <c r="G18" s="8"/>
-      <c r="H18" s="7"/>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H18" s="8"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="7"/>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C22" s="9"/>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C23" s="9"/>
     </row>
   </sheetData>
@@ -2211,22 +2271,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:C14"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="26.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="39.140625" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="8.83203125" style="1"/>
+    <col min="2" max="2" width="26.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="39.1640625" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:3" x14ac:dyDescent="0.2">
       <c r="C1" s="3"/>
     </row>
-    <row r="2" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="16" t="s">
         <v>5</v>
       </c>
@@ -2234,7 +2294,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B3" s="16" t="s">
         <v>0</v>
       </c>
@@ -2242,7 +2302,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B4" s="16" t="s">
         <v>6</v>
       </c>
@@ -2250,7 +2310,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="2:3" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:3" s="7" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B5" s="17" t="s">
         <v>2</v>
       </c>
@@ -2258,7 +2318,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="2:3" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:3" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.15">
       <c r="B6" s="17" t="s">
         <v>7</v>
       </c>
@@ -2266,7 +2326,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="2:3" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:3" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.15">
       <c r="B7" s="17" t="s">
         <v>4</v>
       </c>
@@ -2274,7 +2334,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="2:3" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:3" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.15">
       <c r="B8" s="17" t="s">
         <v>15</v>
       </c>
@@ -2282,10 +2342,10 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:3" x14ac:dyDescent="0.2">
       <c r="C13" s="9"/>
     </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:3" x14ac:dyDescent="0.2">
       <c r="C14" s="9"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adicionada EAP do projeto.
</commit_message>
<xml_diff>
--- a/Artefatos de Documentação/Processo Aplicado/EveRemind/2-Gerencia de Projeto/Templates/Cronograma.xlsx
+++ b/Artefatos de Documentação/Processo Aplicado/EveRemind/2-Gerencia de Projeto/Templates/Cronograma.xlsx
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
   <si>
     <t>Atividade</t>
   </si>
@@ -109,6 +109,9 @@
   </si>
   <si>
     <t>Custo Estimado</t>
+  </si>
+  <si>
+    <t>Gerência de Projetos</t>
   </si>
 </sst>
 </file>
@@ -492,7 +495,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -622,6 +625,43 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -683,10 +723,9 @@
     <xf numFmtId="0" fontId="1" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -732,6 +771,15 @@
     </xf>
     <xf numFmtId="0" fontId="21" fillId="36" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="58">
@@ -1765,10 +1813,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:J23"/>
+  <dimension ref="B1:J29"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1776,232 +1824,303 @@
     <col min="1" max="1" width="8.83203125" style="1"/>
     <col min="2" max="2" width="18.1640625" style="1" customWidth="1"/>
     <col min="3" max="3" width="18.5" style="1" customWidth="1"/>
-    <col min="4" max="4" width="36.33203125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="36.33203125" style="3" customWidth="1"/>
     <col min="5" max="5" width="16.6640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5" style="4" customWidth="1"/>
-    <col min="7" max="9" width="19.83203125" style="4" customWidth="1"/>
+    <col min="6" max="6" width="15.5" style="3" customWidth="1"/>
+    <col min="7" max="9" width="19.83203125" style="3" customWidth="1"/>
     <col min="10" max="10" width="25.5" style="1" customWidth="1"/>
     <col min="11" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="C1" s="3"/>
-      <c r="E1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="6"/>
+      <c r="C1" s="2"/>
+      <c r="E1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="5"/>
     </row>
     <row r="2" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="F2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="G2" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="11" t="s">
+      <c r="H2" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="11" t="s">
+      <c r="I2" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="J2" s="10" t="s">
+      <c r="J2" s="9" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B3" s="2"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="13"/>
+      <c r="B3" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="12"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="12"/>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B4" s="2"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="14"/>
-    </row>
-    <row r="5" spans="2:10" s="7" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B5" s="15"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="14"/>
-    </row>
-    <row r="6" spans="2:10" s="7" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B6" s="15"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
-    </row>
-    <row r="7" spans="2:10" s="7" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B7" s="15"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="14"/>
-    </row>
-    <row r="8" spans="2:10" s="7" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B8" s="15"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
-    </row>
-    <row r="9" spans="2:10" s="7" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B9" s="15"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
-    </row>
-    <row r="10" spans="2:10" s="7" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B10" s="15"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
-    </row>
-    <row r="11" spans="2:10" s="7" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B11" s="15"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="14"/>
-    </row>
-    <row r="12" spans="2:10" s="7" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B12" s="15"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
-    </row>
-    <row r="13" spans="2:10" s="7" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B13" s="15"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14"/>
-    </row>
-    <row r="14" spans="2:10" s="7" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B14" s="15"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="14"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="14"/>
-    </row>
-    <row r="15" spans="2:10" s="7" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B15" s="15"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
-    </row>
-    <row r="16" spans="2:10" s="7" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B16" s="15"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="14"/>
-      <c r="I16" s="14"/>
-      <c r="J16" s="14"/>
-    </row>
-    <row r="17" spans="2:10" s="7" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B17" s="15"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="14"/>
-      <c r="I17" s="14"/>
-      <c r="J17" s="14"/>
-    </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="D18" s="8"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
-      <c r="I18" s="8"/>
-      <c r="J18" s="7"/>
-    </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="C22" s="9"/>
-    </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="C23" s="9"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="13"/>
+    </row>
+    <row r="5" spans="2:10" s="6" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B5" s="18"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="13"/>
+    </row>
+    <row r="6" spans="2:10" s="6" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B6" s="18"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13"/>
+    </row>
+    <row r="7" spans="2:10" s="6" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B7" s="18"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="13"/>
+    </row>
+    <row r="8" spans="2:10" s="6" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B8" s="18"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="13"/>
+    </row>
+    <row r="9" spans="2:10" s="6" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B9" s="18"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="13"/>
+    </row>
+    <row r="10" spans="2:10" s="6" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B10" s="18"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="13"/>
+    </row>
+    <row r="11" spans="2:10" s="6" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B11" s="18"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="13"/>
+    </row>
+    <row r="12" spans="2:10" s="6" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B12" s="19"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="13"/>
+    </row>
+    <row r="13" spans="2:10" s="6" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B13" s="14"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="13"/>
+      <c r="J13" s="13"/>
+    </row>
+    <row r="14" spans="2:10" s="6" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B14" s="14"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="13"/>
+      <c r="J14" s="13"/>
+    </row>
+    <row r="15" spans="2:10" s="6" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B15" s="14"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="13"/>
+    </row>
+    <row r="16" spans="2:10" s="6" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B16" s="14"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="13"/>
+      <c r="J16" s="13"/>
+    </row>
+    <row r="17" spans="2:10" s="6" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B17" s="14"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="13"/>
+      <c r="J17" s="13"/>
+    </row>
+    <row r="18" spans="2:10" s="6" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B18" s="14"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="13"/>
+      <c r="I18" s="13"/>
+      <c r="J18" s="13"/>
+    </row>
+    <row r="19" spans="2:10" s="6" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B19" s="14"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="13"/>
+      <c r="I19" s="13"/>
+      <c r="J19" s="13"/>
+    </row>
+    <row r="20" spans="2:10" s="6" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B20" s="14"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
+      <c r="H20" s="13"/>
+      <c r="I20" s="13"/>
+      <c r="J20" s="13"/>
+    </row>
+    <row r="21" spans="2:10" s="6" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B21" s="14"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
+      <c r="H21" s="13"/>
+      <c r="I21" s="13"/>
+      <c r="J21" s="13"/>
+    </row>
+    <row r="22" spans="2:10" s="6" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B22" s="14"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="13"/>
+      <c r="H22" s="13"/>
+      <c r="I22" s="13"/>
+      <c r="J22" s="13"/>
+    </row>
+    <row r="23" spans="2:10" s="6" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B23" s="14"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
+      <c r="H23" s="13"/>
+      <c r="I23" s="13"/>
+      <c r="J23" s="13"/>
+    </row>
+    <row r="24" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="D24" s="7"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
+      <c r="H24" s="7"/>
+      <c r="I24" s="7"/>
+      <c r="J24" s="6"/>
+    </row>
+    <row r="28" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="C28" s="8"/>
+    </row>
+    <row r="29" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="C29" s="8"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B3:B12"/>
+  </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="D3">
     <cfRule type="cellIs" dxfId="74" priority="74" operator="equal">
@@ -2224,7 +2343,7 @@
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D16">
+  <conditionalFormatting sqref="D16:D22">
     <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
       <formula>2</formula>
     </cfRule>
@@ -2241,7 +2360,7 @@
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D17">
+  <conditionalFormatting sqref="D23">
     <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
       <formula>2</formula>
     </cfRule>
@@ -2284,69 +2403,69 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="C1" s="3"/>
+      <c r="C1" s="2"/>
     </row>
     <row r="2" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="C2" s="17" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="12" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="13" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="2:3" s="7" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B5" s="17" t="s">
+    <row r="5" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B5" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="2:3" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.15">
-      <c r="B6" s="17" t="s">
+    <row r="6" spans="2:3" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.15">
+      <c r="B6" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="13" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="2:3" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.15">
-      <c r="B7" s="17" t="s">
+    <row r="7" spans="2:3" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.15">
+      <c r="B7" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="13" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="2:3" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.15">
-      <c r="B8" s="17" t="s">
+    <row r="8" spans="2:3" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.15">
+      <c r="B8" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="C8" s="13" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="C13" s="9"/>
+      <c r="C13" s="8"/>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="C14" s="9"/>
+      <c r="C14" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.31496062992125984" right="0.35433070866141736" top="0.98425196850393704" bottom="0.98425196850393704" header="0.51181102362204722" footer="0.51181102362204722"/>

</xml_diff>